<commit_message>
added budget and chatbot controller
</commit_message>
<xml_diff>
--- a/tmp/budget-summary.xlsx
+++ b/tmp/budget-summary.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Item</t>
   </si>
@@ -22,22 +22,25 @@
     <t>Your name</t>
   </si>
   <si>
-    <t>Femi</t>
+    <t>John Doe</t>
   </si>
   <si>
     <t>Booking Artist</t>
   </si>
   <si>
-    <t>hi</t>
+    <t>Wizkid</t>
   </si>
   <si>
     <t>Location</t>
   </si>
   <si>
-    <t>there would be 2</t>
-  </si>
-  <si>
-    <t>Gold</t>
+    <t>London UK</t>
+  </si>
+  <si>
+    <t>Capacity</t>
+  </si>
+  <si>
+    <t>2025-06-19</t>
   </si>
   <si>
     <t>Currency</t>
@@ -47,6 +50,72 @@
   </si>
   <si>
     <t>Ticket Tiers</t>
+  </si>
+  <si>
+    <t>Regular (1000 @ 100)</t>
+  </si>
+  <si>
+    <t>Venue</t>
+  </si>
+  <si>
+    <t>Venue barricade</t>
+  </si>
+  <si>
+    <t>Box office Personnel</t>
+  </si>
+  <si>
+    <t>Ticket Printing</t>
+  </si>
+  <si>
+    <t>Ushers</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>Lighting Technician</t>
+  </si>
+  <si>
+    <t>Audio Technician</t>
+  </si>
+  <si>
+    <t>Stage Hands</t>
+  </si>
+  <si>
+    <t>Medical Cost</t>
+  </si>
+  <si>
+    <t>Stage</t>
+  </si>
+  <si>
+    <t>Lights?</t>
+  </si>
+  <si>
+    <t>Backline</t>
+  </si>
+  <si>
+    <t>Sound</t>
+  </si>
+  <si>
+    <t>Outdoor Posters</t>
+  </si>
+  <si>
+    <t>Radio Advertising</t>
+  </si>
+  <si>
+    <t>Artist Fee</t>
+  </si>
+  <si>
+    <t>Digital Ads</t>
+  </si>
+  <si>
+    <t>Flights</t>
+  </si>
+  <si>
+    <t>Accommodation</t>
+  </si>
+  <si>
+    <t>Catering</t>
   </si>
   <si>
     <t>Gross Revenue</t>
@@ -435,7 +504,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B36"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
@@ -474,40 +543,233 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B5" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="B13" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="1">
+        <v>105000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="1">
+        <v>-5000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>